<commit_message>
delphi changed? source folder for cpp/hpp files
</commit_message>
<xml_diff>
--- a/delphi.xlsx
+++ b/delphi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1112d360afa47f28/Documents/P3AT_LY-P/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\OneDrive\Documents\AzureGit%20-%20P3AT%20Team1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{526167E9-8ABC-46E4-8F75-EB58342FEB77}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{D7FB5090-6409-4F8E-8EE3-D18E0782404F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>